<commit_message>
updating excel file for revisions to wc-lang
</commit_message>
<xml_diff>
--- a/tests/fixtures/understand_rates_model.xlsx
+++ b/tests/fixtures/understand_rates_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,16 +19,16 @@
     <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Biomass components" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Biomass reactions" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Biomass components" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Parameters" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Stop conditions" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="References" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Database references" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$106</definedName>
     <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
@@ -41,24 +41,56 @@
     <definedName function="false" hidden="true" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$60</definedName>
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$F$3</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Model!$A$1:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Taxon!$A$1:$A$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$60</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$60</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$E$106</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$E$106</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$E$106</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Observables!$A$1:$D$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Observables!$A$1:$D$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Observables!$A$1:$D$12</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Functions!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$38</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$38</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$38</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$38</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$38</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$38</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass reactions'!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Biomass components'!$A$1:$G$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Stop conditions'!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$Q$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -70,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="95">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -114,169 +146,169 @@
     <t xml:space="preserve">Algorithm</t>
   </si>
   <si>
+    <t xml:space="preserve">Objective function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metabolism_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metabolism_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cytosol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracellular space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empirical formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molecular weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adenosine- 5’-diphosphate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/C10H15N5O10P2/c11-8-5-9(13-2-12-8)15(3-14-5)10-7(17)6(16)4(24-10)1-23-27(21,22)25-26(18,19)20/h2-4,6-7,10,16-17H,1H2,(H,21,22)(H2,11,12,13)(H2,18,19,20)/t4-,6-,7-,10-/m1/s1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10H15N5O10P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metabolite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alanine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InChI=1S/C3H7NO2/c1-2(4)3(5)6/h2H,4H2,1H3,(H,5,6)/t2-/m0/s1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3H7NO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Compartment</t>
   </si>
   <si>
+    <t xml:space="preserve">A[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">molecules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transfer_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A[e] ==&gt; A[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transfer_B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B[e] ==&gt; B[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biomass reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objective function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metabolism_A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metabolism_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cytosol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extracellular space</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empirical formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molecular weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adenosine- 5’-diphosphate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InChI=1S/C10H15N5O10P2/c11-8-5-9(13-2-12-8)15(3-14-5)10-7(17)6(16)4(24-10)1-23-27(21,22)25-26(18,19)20/h2-4,6-7,10,16-17H,1H2,(H,21,22)(H2,11,12,13)(H2,18,19,20)/t4-,6-,7-,10-/m1/s1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10H15N5O10P2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metabolite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alanine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InChI=1S/C3H7NO2/c1-2(4)3(5)6/h2H,4H2,1H3,(H,5,6)/t2-/m0/s1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3H7NO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">molecules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transfer_A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A[e] ==&gt; A[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transfer_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B[e] ==&gt; B[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forward</t>
   </si>
   <si>
     <t xml:space="preserve">Coefficient</t>
@@ -715,10 +747,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3846153846154"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6315789473684"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -730,19 +762,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
@@ -753,14 +785,14 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -773,14 +805,14 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -1206,27 +1238,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>10</v>
@@ -1237,13 +1269,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1252,13 +1284,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1598,14 +1630,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1621,23 +1653,17 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1"/>
+  <autoFilter ref="A1:E1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1654,14 +1680,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1677,17 +1703,23 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:G1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1733,10 +1765,10 @@
         <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>10</v>
@@ -1858,7 +1890,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -1917,7 +1949,7 @@
         <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>82</v>
@@ -2000,16 +2032,16 @@
         <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>94</v>
@@ -2091,19 +2123,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2121,48 +2153,38 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H3"/>
+  <autoFilter ref="A1:F3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2202,7 +2224,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -2213,10 +2235,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>1E-015</v>
@@ -2226,10 +2248,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1E-010</v>
@@ -2278,19 +2300,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
@@ -2301,16 +2323,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>427.201122</v>
@@ -2319,23 +2341,23 @@
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>89.09318</v>
@@ -2344,23 +2366,23 @@
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>427.201122</v>
@@ -2369,23 +2391,23 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>89.09318</v>
@@ -2394,7 +2416,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -3024,7 +3046,7 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -3034,8 +3056,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3046,10 +3068,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
@@ -3060,68 +3082,68 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3157,20 +3179,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -3181,78 +3203,78 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>1E-006</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>0.005</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>500000</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>1.67E-007</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>100</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -3287,9 +3309,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3301,7 +3323,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
@@ -3414,7 +3436,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
refactoring units similar to wc_lang
</commit_message>
<xml_diff>
--- a/tests/fixtures/understand_rates_model.xlsx
+++ b/tests/fixtures/understand_rates_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" firstSheet="6" activeTab="19"/>
+    <workbookView windowWidth="20295" windowHeight="6840" tabRatio="993" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="156">
   <si>
     <t>Id</t>
   </si>
@@ -218,145 +218,148 @@
     <t>Temperature units</t>
   </si>
   <si>
+    <t>degC</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>pH units</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Evidence</t>
+  </si>
+  <si>
+    <t>Interpretations</t>
+  </si>
+  <si>
+    <t>metabolism_A</t>
+  </si>
+  <si>
+    <t>stochastic_simulation_algorithm</t>
+  </si>
+  <si>
+    <t>metabolism_B</t>
+  </si>
+  <si>
+    <t>Biological type</t>
+  </si>
+  <si>
+    <t>Physical type</t>
+  </si>
+  <si>
+    <t>Geometry</t>
+  </si>
+  <si>
+    <t>Parent compartment</t>
+  </si>
+  <si>
+    <t>Mass units</t>
+  </si>
+  <si>
+    <t>Initial volume distribution</t>
+  </si>
+  <si>
+    <t>Initial volume mean</t>
+  </si>
+  <si>
+    <t>Initial volume standard deviation</t>
+  </si>
+  <si>
+    <t>Initial volume units</t>
+  </si>
+  <si>
+    <t>Initial density</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Cytosol</t>
+  </si>
+  <si>
+    <t>cellular_compartment</t>
+  </si>
+  <si>
+    <t>fluid_compartment</t>
+  </si>
+  <si>
+    <t>3D_compartment</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>normal_distribution</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>density_c</t>
+  </si>
+  <si>
+    <t>Extracellular space</t>
+  </si>
+  <si>
+    <t>extracellular_compartment</t>
+  </si>
+  <si>
+    <t>density_e</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Empirical formula</t>
+  </si>
+  <si>
+    <t>Molecular weight</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>adenosine- 5’-diphosphate</t>
+  </si>
+  <si>
+    <t>InChI=1S/C10H15N5O10P2/c11-8-5-9(13-2-12-8)15(3-14-5)10-7(17)6(16)4(24-10)1-23-27(21,22)25-26(18,19)20/h2-4,6-7,10,16-17H,1H2,(H,21,22)(H2,11,12,13)(H2,18,19,20)/t4-,6-,7-,10-/m1/s1</t>
+  </si>
+  <si>
+    <t>C10H15N5O10P2</t>
+  </si>
+  <si>
+    <t>metabolite</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>alanine</t>
+  </si>
+  <si>
+    <t>InChI=1S/C3H7NO2/c1-2(4)3(5)6/h2H,4H2,1H3,(H,5,6)/t2-/m0/s1</t>
+  </si>
+  <si>
+    <t>C3H7NO2</t>
+  </si>
+  <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>pH units</t>
-  </si>
-  <si>
-    <t>dimensionless</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>Evidence</t>
-  </si>
-  <si>
-    <t>Interpretations</t>
-  </si>
-  <si>
-    <t>metabolism_A</t>
-  </si>
-  <si>
-    <t>stochastic_simulation_algorithm</t>
-  </si>
-  <si>
-    <t>metabolism_B</t>
-  </si>
-  <si>
-    <t>Biological type</t>
-  </si>
-  <si>
-    <t>Physical type</t>
-  </si>
-  <si>
-    <t>Geometry</t>
-  </si>
-  <si>
-    <t>Parent compartment</t>
-  </si>
-  <si>
-    <t>Mass units</t>
-  </si>
-  <si>
-    <t>Initial volume distribution</t>
-  </si>
-  <si>
-    <t>Initial volume mean</t>
-  </si>
-  <si>
-    <t>Initial volume standard deviation</t>
-  </si>
-  <si>
-    <t>Initial volume units</t>
-  </si>
-  <si>
-    <t>Initial density</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Cytosol</t>
-  </si>
-  <si>
-    <t>cellular_compartment</t>
-  </si>
-  <si>
-    <t>fluid_compartment</t>
-  </si>
-  <si>
-    <t>3D_compartment</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>normal_distribution</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>density_c</t>
-  </si>
-  <si>
-    <t>Extracellular space</t>
-  </si>
-  <si>
-    <t>extracellular_compartment</t>
-  </si>
-  <si>
-    <t>density_e</t>
-  </si>
-  <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>Empirical formula</t>
-  </si>
-  <si>
-    <t>Molecular weight</t>
-  </si>
-  <si>
-    <t>Charge</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>adenosine- 5’-diphosphate</t>
-  </si>
-  <si>
-    <t>InChI=1S/C10H15N5O10P2/c11-8-5-9(13-2-12-8)15(3-14-5)10-7(17)6(16)4(24-10)1-23-27(21,22)25-26(18,19)20/h2-4,6-7,10,16-17H,1H2,(H,21,22)(H2,11,12,13)(H2,18,19,20)/t4-,6-,7-,10-/m1/s1</t>
-  </si>
-  <si>
-    <t>C10H15N5O10P2</t>
-  </si>
-  <si>
-    <t>metabolite</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>alanine</t>
-  </si>
-  <si>
-    <t>InChI=1S/C3H7NO2/c1-2(4)3(5)6/h2H,4H2,1H3,(H,5,6)/t2-/m0/s1</t>
-  </si>
-  <si>
-    <t>C3H7NO2</t>
   </si>
   <si>
     <t>D</t>
@@ -617,9 +620,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -653,13 +656,76 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -674,7 +740,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -687,6 +753,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -694,40 +776,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -747,55 +797,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -816,7 +819,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -828,25 +927,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -858,19 +939,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,73 +975,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -966,37 +993,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,6 +1010,24 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1026,21 +1047,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1051,15 +1057,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1090,6 +1087,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1098,148 +1110,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1823,10 +1826,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>15</v>
@@ -1846,10 +1849,10 @@
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>52</v>
@@ -1857,10 +1860,10 @@
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
@@ -1906,25 +1909,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>15</v>
@@ -1944,38 +1947,38 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="15.1" customHeight="1" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E3" s="1" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2021,19 +2024,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>15</v>
@@ -3066,38 +3069,36 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>114</v>
+      </c>
       <c r="F2" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3136,19 +3137,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>15</v>
@@ -3202,13 +3203,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>15</v>
@@ -3262,16 +3263,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>15</v>
@@ -3334,13 +3335,13 @@
         <v>61</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>15</v>
@@ -4374,7 +4375,7 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D2" s="1">
         <v>100</v>
@@ -4385,7 +4386,7 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D3" s="1">
         <v>100</v>
@@ -4396,7 +4397,7 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D4" s="1">
         <v>0.3</v>
@@ -4407,7 +4408,7 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1">
         <v>0.3</v>
@@ -4418,30 +4419,30 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4452,7 +4453,7 @@
         <v>1100</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4463,18 +4464,18 @@
         <v>1000</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D10" s="6">
         <v>6.02214075862e+23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -4513,10 +4514,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>15</v>
@@ -4570,22 +4571,22 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>22</v>
@@ -4600,22 +4601,22 @@
         <v>26</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>15</v>
@@ -4669,19 +4670,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>15</v>
@@ -4802,7 +4803,7 @@
   <sheetPr/>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -4823,46 +4824,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>61</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>15</v>
@@ -4886,10 +4887,10 @@
   <sheetPr/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A6" sqref="A6:B6"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
@@ -6319,7 +6320,7 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>63</v>
@@ -6342,7 +6343,7 @@
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>68</v>
@@ -6405,13 +6406,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>15</v>
@@ -6431,7 +6432,7 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>62</v>
@@ -6440,12 +6441,12 @@
         <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>62</v>
@@ -6454,12 +6455,12 @@
         <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>67</v>
@@ -6468,12 +6469,12 @@
         <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>67</v>
@@ -6482,35 +6483,35 @@
         <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -6558,19 +6559,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>15</v>
@@ -6590,10 +6591,10 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>51</v>
@@ -6602,15 +6603,15 @@
         <v>1e-6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="15.1" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>51</v>
@@ -6619,15 +6620,15 @@
         <v>0.005</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="15.1" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>51</v>
@@ -6636,15 +6637,15 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="15.1" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>51</v>
@@ -6653,15 +6654,15 @@
         <v>500000</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="15.1" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>51</v>
@@ -6670,15 +6671,15 @@
         <v>1.67e-7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="15.1" customHeight="1" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>51</v>
@@ -6687,7 +6688,7 @@
         <v>100</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -6729,10 +6730,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>15</v>

</xml_diff>